<commit_message>
Updated on 14march 18:23
</commit_message>
<xml_diff>
--- a/src/main/resources/Q11-Hosting.xlsx
+++ b/src/main/resources/Q11-Hosting.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2419" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2864" uniqueCount="281">
   <si>
     <t xml:space="preserve">By Default </t>
   </si>
@@ -842,6 +842,87 @@
   </si>
   <si>
     <t>cGoBk183</t>
+  </si>
+  <si>
+    <t>Prometheus95894</t>
+  </si>
+  <si>
+    <t>ODuYZ712</t>
+  </si>
+  <si>
+    <t>Linux Hosting New Gold ( for phoenix975lr.com )</t>
+  </si>
+  <si>
+    <t>Prometheus93178</t>
+  </si>
+  <si>
+    <t>f6Jyc621</t>
+  </si>
+  <si>
+    <t>Linux Hosting New Gold ( for phoenix916gn.com )</t>
+  </si>
+  <si>
+    <t>Prometheus0811</t>
+  </si>
+  <si>
+    <t>4pHeb043</t>
+  </si>
+  <si>
+    <t>Linux Hosting New Gold ( for phoenix582fp.onmicrosoft.com )</t>
+  </si>
+  <si>
+    <t>Prometheus6455</t>
+  </si>
+  <si>
+    <t>v5AWt805</t>
+  </si>
+  <si>
+    <t>Linux Hosting New Gold ( for phoenix796dn.onmicrosoft.com )</t>
+  </si>
+  <si>
+    <t>Prometheus0536</t>
+  </si>
+  <si>
+    <t>2lnRw551</t>
+  </si>
+  <si>
+    <t>Linux Hosting New Gold ( for phoenix885ys.onmicrosoft.com )</t>
+  </si>
+  <si>
+    <t>Prometheus3793</t>
+  </si>
+  <si>
+    <t>UEgDD941</t>
+  </si>
+  <si>
+    <t>Prometheus9403</t>
+  </si>
+  <si>
+    <t>zbwjE678</t>
+  </si>
+  <si>
+    <t>Linux Hosting New Gold ( for phoenix435bb.onmicrosoft.com )</t>
+  </si>
+  <si>
+    <t>Prometheus9557</t>
+  </si>
+  <si>
+    <t>RmcfD191</t>
+  </si>
+  <si>
+    <t>Linux Hosting New Gold ( for phoenix880sr.onmicrosoft.com )</t>
+  </si>
+  <si>
+    <t>Prometheus8297</t>
+  </si>
+  <si>
+    <t>WXf43538</t>
+  </si>
+  <si>
+    <t>Prometheus0652</t>
+  </si>
+  <si>
+    <t>Yhaxy774</t>
   </si>
 </sst>
 </file>
@@ -992,7 +1073,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1049,6 +1130,14 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -3079,7 +3168,7 @@
         <v>75</v>
       </c>
       <c r="K4" s="25" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
@@ -3096,7 +3185,7 @@
         <v>79</v>
       </c>
       <c r="K5" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
@@ -3127,7 +3216,7 @@
         <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
         <v>45</v>
@@ -3454,10 +3543,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>233</v>
+        <v>259</v>
       </c>
       <c r="B27" t="s">
-        <v>233</v>
+        <v>259</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>37</v>
@@ -7701,7 +7790,7 @@
         <v>75</v>
       </c>
       <c r="K4" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -7718,7 +7807,7 @@
         <v>79</v>
       </c>
       <c r="K5" t="s">
-        <v>209</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -7749,7 +7838,7 @@
         <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
         <v>45</v>
@@ -8061,10 +8150,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>210</v>
+        <v>276</v>
       </c>
       <c r="B27" t="s">
-        <v>210</v>
+        <v>276</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>37</v>

</xml_diff>